<commit_message>
Updating Sheet to create a new branch
</commit_message>
<xml_diff>
--- a/Excel/DesignSheet_V0.1.0.xlsx
+++ b/Excel/DesignSheet_V0.1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\AutoSheet\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73766BB-4B5B-4C1B-8D3C-A4F425A73C41}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28960C4C-C9D9-4900-94E3-646F29F13C79}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StormDesign" sheetId="3" r:id="rId1"/>
@@ -627,25 +627,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC95A26-B4BE-4805-866F-7CD05B06D4A2}">
   <dimension ref="E1:BE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AM3" sqref="AM3"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="9.140625" style="12"/>
-    <col min="7" max="7" width="23.42578125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="10"/>
-    <col min="9" max="9" width="11.85546875" style="10" customWidth="1"/>
-    <col min="10" max="23" width="9.140625" style="12"/>
-    <col min="24" max="24" width="10.5703125" style="12" customWidth="1"/>
-    <col min="25" max="25" width="11.140625" style="12" customWidth="1"/>
-    <col min="26" max="37" width="9.140625" style="12"/>
-    <col min="38" max="38" width="11.85546875" style="12" customWidth="1"/>
-    <col min="39" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="6" width="9.109375" style="12"/>
+    <col min="7" max="7" width="23.44140625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="10"/>
+    <col min="9" max="9" width="11.88671875" style="10" customWidth="1"/>
+    <col min="10" max="23" width="9.109375" style="12"/>
+    <col min="24" max="24" width="10.5546875" style="12" customWidth="1"/>
+    <col min="25" max="25" width="11.109375" style="12" customWidth="1"/>
+    <col min="26" max="37" width="9.109375" style="12"/>
+    <col min="38" max="38" width="11.88671875" style="12" customWidth="1"/>
+    <col min="39" max="16384" width="9.109375" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:57" x14ac:dyDescent="0.25">
+    <row r="1" spans="5:57" x14ac:dyDescent="0.3">
       <c r="H1" s="13" t="s">
         <v>30</v>
       </c>
@@ -729,7 +729,7 @@
       <c r="BD1" s="13"/>
       <c r="BE1" s="13"/>
     </row>
-    <row r="2" spans="5:57" s="10" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="5:57" s="10" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E2" s="10" t="s">
         <v>61</v>
       </c>
@@ -877,7 +877,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="5:57" x14ac:dyDescent="0.25">
+    <row r="3" spans="5:57" x14ac:dyDescent="0.3">
       <c r="E3" s="12" t="str">
         <f>_xlfn.CONCAT(H3,"-",I3)</f>
         <v>192-191</v>
@@ -898,12 +898,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AW1:AZ1"/>
-    <mergeCell ref="BA1:BE1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="AM1:AV1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="X1:X2"/>
     <mergeCell ref="Y1:Y2"/>
@@ -914,6 +908,12 @@
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="W1:W2"/>
+    <mergeCell ref="AW1:AZ1"/>
+    <mergeCell ref="BA1:BE1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AM1:AV1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -923,18 +923,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="14.85546875" style="1"/>
-    <col min="4" max="4" width="14.85546875" style="9"/>
-    <col min="5" max="16384" width="14.85546875" style="1"/>
+    <col min="1" max="3" width="14.88671875" style="1"/>
+    <col min="4" max="4" width="14.88671875" style="9"/>
+    <col min="5" max="16384" width="14.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -978,7 +978,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <f>PipeDataXlIn!A2</f>
         <v>27926</v>
@@ -1024,7 +1024,7 @@
         <v>103.25000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>PipeDataXlIn!A3</f>
         <v>27952</v>
@@ -1070,7 +1070,7 @@
         <v>102.55000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f>PipeDataXlIn!A4</f>
         <v>27960</v>
@@ -1116,7 +1116,7 @@
         <v>102.02500000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f>PipeDataXlIn!A5</f>
         <v>27986</v>
@@ -1162,7 +1162,7 @@
         <v>101.32500000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f>PipeDataXlIn!A6</f>
         <v>28012</v>
@@ -1208,7 +1208,7 @@
         <v>100.62500000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f>PipeDataXlIn!A7</f>
         <v>28038</v>
@@ -1254,7 +1254,7 @@
         <v>100.10000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f>PipeDataXlIn!A8</f>
         <v>28064</v>
@@ -1300,7 +1300,7 @@
         <v>99.4</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F9" s="2"/>
       <c r="I9" s="8">
         <v>100</v>
@@ -1311,7 +1311,7 @@
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F10" s="2"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -1320,7 +1320,7 @@
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F11" s="2"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -1329,7 +1329,7 @@
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F12" s="2"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -1338,7 +1338,7 @@
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F13" s="2"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -1347,7 +1347,7 @@
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F14" s="2"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
@@ -1356,7 +1356,7 @@
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F15" s="2"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
@@ -1365,7 +1365,7 @@
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F16" s="2"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -1374,7 +1374,7 @@
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
     </row>
-    <row r="17" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
@@ -1382,7 +1382,7 @@
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
     </row>
-    <row r="18" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -1390,7 +1390,7 @@
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
     </row>
-    <row r="19" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
@@ -1398,7 +1398,7 @@
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
     </row>
-    <row r="20" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -1406,7 +1406,7 @@
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
     </row>
-    <row r="21" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -1414,7 +1414,7 @@
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
     </row>
-    <row r="22" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -1422,7 +1422,7 @@
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
     </row>
-    <row r="23" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -1430,7 +1430,7 @@
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
     </row>
-    <row r="24" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
@@ -1438,7 +1438,7 @@
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
     </row>
-    <row r="25" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -1446,7 +1446,7 @@
       <c r="M25" s="8"/>
       <c r="N25" s="8"/>
     </row>
-    <row r="26" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
@@ -1454,7 +1454,7 @@
       <c r="M26" s="8"/>
       <c r="N26" s="8"/>
     </row>
-    <row r="27" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
@@ -1462,7 +1462,7 @@
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
     </row>
-    <row r="28" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
@@ -1470,7 +1470,7 @@
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
     </row>
-    <row r="29" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
@@ -1478,7 +1478,7 @@
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
     </row>
-    <row r="30" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
@@ -1486,7 +1486,7 @@
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
     </row>
-    <row r="31" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
@@ -1494,7 +1494,7 @@
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
     </row>
-    <row r="32" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
@@ -1502,7 +1502,7 @@
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
     </row>
-    <row r="33" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
@@ -1510,7 +1510,7 @@
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
     </row>
-    <row r="34" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
@@ -1518,7 +1518,7 @@
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
     </row>
-    <row r="35" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
@@ -1526,7 +1526,7 @@
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
     </row>
-    <row r="36" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
@@ -1534,7 +1534,7 @@
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
     </row>
-    <row r="37" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
@@ -1542,7 +1542,7 @@
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
     </row>
-    <row r="38" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
@@ -1550,7 +1550,7 @@
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
     </row>
-    <row r="39" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
@@ -1558,7 +1558,7 @@
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
     </row>
-    <row r="40" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="9:14" x14ac:dyDescent="0.3">
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
@@ -1580,20 +1580,20 @@
       <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="16.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="9.140625" style="7"/>
-    <col min="6" max="6" width="16.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="16.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="1"/>
+    <col min="5" max="5" width="9.109375" style="7"/>
+    <col min="6" max="6" width="16.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>27926</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>-5.4249999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>27952</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>-7.5249999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>27960</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>-9.125</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>27986</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>-11.225</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>28012</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>-13.324999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>28038</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>-14.924999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>28064</v>
       </c>
@@ -1801,25 +1801,25 @@
         <v>-17.024999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F15" s="8"/>
     </row>
   </sheetData>

</xml_diff>